<commit_message>
Add proposed priorities to spreadsheet
</commit_message>
<xml_diff>
--- a/schema/schema.xlsx
+++ b/schema/schema.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1344" uniqueCount="609">
   <si>
     <t>Exemption</t>
   </si>
@@ -1958,6 +1958,18 @@
   </si>
   <si>
     <t>RWG063109</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -2774,11 +2786,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:N96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="44.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2789,12 +2803,14 @@
     <col min="4" max="4" width="82.6640625" style="4" customWidth="1"/>
     <col min="5" max="7" width="25.83203125" style="6" customWidth="1"/>
     <col min="8" max="9" width="23.1640625" style="6" customWidth="1"/>
-    <col min="10" max="12" width="44.6640625" style="6"/>
-    <col min="13" max="13" width="81.6640625" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="44.6640625" style="6"/>
+    <col min="10" max="11" width="44.6640625" style="6"/>
+    <col min="12" max="12" width="8.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.6640625" style="6"/>
+    <col min="14" max="14" width="81.6640625" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="44.6640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1">
+    <row r="1" spans="1:14" s="11" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -2829,13 +2845,16 @@
         <v>179</v>
       </c>
       <c r="L1" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="M1" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="45">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="45">
       <c r="A2" s="3" t="s">
         <v>114</v>
       </c>
@@ -2870,13 +2889,16 @@
         <v>159</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>135</v>
+        <v>606</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="3" spans="1:14" ht="30">
       <c r="A3" s="3" t="s">
         <v>115</v>
       </c>
@@ -2910,14 +2932,17 @@
       <c r="K3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="L3" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30">
       <c r="A4" s="3" t="s">
         <v>116</v>
       </c>
@@ -2952,13 +2977,16 @@
         <v>188</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>135</v>
+        <v>606</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N4" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30">
       <c r="A5" s="3" t="s">
         <v>117</v>
       </c>
@@ -2993,13 +3021,16 @@
         <v>188</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>135</v>
+        <v>606</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" ht="75">
+      <c r="N5" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="75">
       <c r="A6" s="3" t="s">
         <v>118</v>
       </c>
@@ -3039,8 +3070,11 @@
       <c r="M6" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" ht="120">
+      <c r="N6" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="120">
       <c r="A7" s="3" t="s">
         <v>601</v>
       </c>
@@ -3075,13 +3109,16 @@
         <v>135</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>135</v>
+        <v>607</v>
       </c>
       <c r="M7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N7" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="8" spans="1:14" ht="75">
       <c r="A8" s="3" t="s">
         <v>119</v>
       </c>
@@ -3116,13 +3153,16 @@
         <v>135</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="9" spans="1:14" ht="30">
       <c r="A9" s="3" t="s">
         <v>120</v>
       </c>
@@ -3156,14 +3196,17 @@
       <c r="K9" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="L9" s="6" t="s">
+      <c r="L9" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="10" spans="1:14" ht="30">
       <c r="A10" s="3" t="s">
         <v>121</v>
       </c>
@@ -3203,8 +3246,11 @@
       <c r="M10" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N10" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30">
       <c r="A11" s="3" t="s">
         <v>122</v>
       </c>
@@ -3239,13 +3285,16 @@
         <v>135</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M11" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N11" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="12" spans="1:14" ht="30">
       <c r="A12" s="3" t="s">
         <v>123</v>
       </c>
@@ -3283,10 +3332,13 @@
         <v>135</v>
       </c>
       <c r="M12" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="13" spans="1:14" ht="75">
       <c r="A13" s="3" t="s">
         <v>98</v>
       </c>
@@ -3321,13 +3373,16 @@
         <v>135</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N13" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="14" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="14" spans="1:14" ht="75">
       <c r="A14" s="3" t="s">
         <v>99</v>
       </c>
@@ -3362,13 +3417,16 @@
         <v>135</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M14" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="15" spans="1:14" ht="60">
       <c r="A15" s="3" t="s">
         <v>100</v>
       </c>
@@ -3403,13 +3461,16 @@
         <v>296</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="6" customFormat="1" ht="180">
+    <row r="16" spans="1:14" ht="180">
       <c r="A16" s="3" t="s">
         <v>101</v>
       </c>
@@ -3444,13 +3505,16 @@
         <v>135</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="6" customFormat="1" ht="165">
+    <row r="17" spans="1:14" ht="165">
       <c r="A17" s="3" t="s">
         <v>102</v>
       </c>
@@ -3485,13 +3549,16 @@
         <v>135</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M17" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="18" spans="1:14" ht="45">
       <c r="A18" s="3" t="s">
         <v>103</v>
       </c>
@@ -3526,13 +3593,16 @@
         <v>292</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M18" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="19" spans="1:14" ht="30">
       <c r="A19" s="3" t="s">
         <v>104</v>
       </c>
@@ -3567,13 +3637,16 @@
         <v>292</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M19" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="20" spans="1:14" ht="60">
       <c r="A20" s="3" t="s">
         <v>105</v>
       </c>
@@ -3608,13 +3681,16 @@
         <v>292</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M20" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="6" customFormat="1" ht="120">
+    <row r="21" spans="1:14" ht="120">
       <c r="A21" s="3" t="s">
         <v>106</v>
       </c>
@@ -3648,14 +3724,17 @@
       <c r="K21" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="M21" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="22" spans="1:14" ht="30">
       <c r="A22" s="3" t="s">
         <v>107</v>
       </c>
@@ -3690,13 +3769,16 @@
         <v>135</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M22" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="23" spans="1:14" ht="45">
       <c r="A23" s="3" t="s">
         <v>108</v>
       </c>
@@ -3731,13 +3813,16 @@
         <v>135</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M23" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N23" s="1" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="24" spans="1:14" ht="45">
       <c r="A24" s="3" t="s">
         <v>109</v>
       </c>
@@ -3772,13 +3857,16 @@
         <v>135</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M24" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="25" spans="1:14" ht="60">
       <c r="A25" s="3" t="s">
         <v>110</v>
       </c>
@@ -3813,13 +3901,16 @@
         <v>135</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="26" spans="1:14" ht="30">
       <c r="A26" s="3" t="s">
         <v>111</v>
       </c>
@@ -3857,10 +3948,13 @@
         <v>135</v>
       </c>
       <c r="M26" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N26" s="1" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="27" spans="1:14" ht="30">
       <c r="A27" s="3" t="s">
         <v>112</v>
       </c>
@@ -3898,10 +3992,13 @@
         <v>135</v>
       </c>
       <c r="M27" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N27" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="28" spans="1:14" ht="60">
       <c r="A28" s="3" t="s">
         <v>113</v>
       </c>
@@ -3936,13 +4033,16 @@
         <v>135</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N28" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="6" customFormat="1" ht="120">
+    <row r="29" spans="1:14" ht="120">
       <c r="A29" s="3" t="s">
         <v>433</v>
       </c>
@@ -3977,13 +4077,16 @@
         <v>135</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>135</v>
+        <v>607</v>
       </c>
       <c r="M29" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N29" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="30" spans="1:14" ht="30">
       <c r="A30" s="3" t="s">
         <v>82</v>
       </c>
@@ -4018,13 +4121,16 @@
         <v>188</v>
       </c>
       <c r="L30" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="31" spans="1:14" ht="30">
       <c r="A31" s="3" t="s">
         <v>83</v>
       </c>
@@ -4058,14 +4164,17 @@
       <c r="K31" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="L31" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="M31" s="1" t="s">
+      <c r="L31" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N31" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="6" customFormat="1" ht="90">
+    <row r="32" spans="1:14" ht="90">
       <c r="A32" s="3" t="s">
         <v>84</v>
       </c>
@@ -4100,13 +4209,16 @@
         <v>135</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M32" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N32" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="33" spans="1:14" ht="60">
       <c r="A33" s="3" t="s">
         <v>85</v>
       </c>
@@ -4141,13 +4253,16 @@
         <v>135</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M33" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N33" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="34" spans="1:14" ht="30">
       <c r="A34" s="3" t="s">
         <v>86</v>
       </c>
@@ -4182,13 +4297,16 @@
         <v>135</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M34" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N34" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="35" spans="1:14" ht="75">
       <c r="A35" s="3" t="s">
         <v>87</v>
       </c>
@@ -4223,13 +4341,16 @@
         <v>210</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N35" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="36" spans="1:14" ht="75">
       <c r="A36" s="3" t="s">
         <v>88</v>
       </c>
@@ -4264,13 +4385,16 @@
         <v>210</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M36" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N36" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="37" spans="1:14" ht="60">
       <c r="A37" s="3" t="s">
         <v>89</v>
       </c>
@@ -4305,13 +4429,16 @@
         <v>188</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M37" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N37" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="38" spans="1:14" ht="30">
       <c r="A38" s="3" t="s">
         <v>90</v>
       </c>
@@ -4346,13 +4473,16 @@
         <v>135</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M38" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N38" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="39" spans="1:14" ht="45">
       <c r="A39" s="3" t="s">
         <v>91</v>
       </c>
@@ -4387,13 +4517,16 @@
         <v>135</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M39" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N39" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="40" spans="1:14" ht="45">
       <c r="A40" s="3" t="s">
         <v>92</v>
       </c>
@@ -4428,13 +4561,16 @@
         <v>188</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M40" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N40" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="41" spans="1:14" ht="45">
       <c r="A41" s="3" t="s">
         <v>93</v>
       </c>
@@ -4469,13 +4605,16 @@
         <v>135</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M41" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N41" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="42" spans="1:14" ht="30">
       <c r="A42" s="3" t="s">
         <v>94</v>
       </c>
@@ -4510,13 +4649,16 @@
         <v>188</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M42" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N42" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="43" spans="1:14" ht="60">
       <c r="A43" s="3" t="s">
         <v>95</v>
       </c>
@@ -4551,13 +4693,16 @@
         <v>230</v>
       </c>
       <c r="L43" s="1" t="s">
-        <v>135</v>
+        <v>606</v>
       </c>
       <c r="M43" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N43" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="44" spans="1:14" ht="30">
       <c r="A44" s="3" t="s">
         <v>96</v>
       </c>
@@ -4595,10 +4740,13 @@
         <v>135</v>
       </c>
       <c r="M44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N44" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="6" customFormat="1">
+    <row r="45" spans="1:14">
       <c r="A45" s="3" t="s">
         <v>97</v>
       </c>
@@ -4633,13 +4781,16 @@
         <v>135</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N45" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="46" spans="1:14" ht="75">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
@@ -4674,13 +4825,16 @@
         <v>135</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N46" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="47" spans="1:14" ht="45">
       <c r="A47" s="3" t="s">
         <v>81</v>
       </c>
@@ -4715,13 +4869,16 @@
         <v>135</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M47" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N47" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="48" spans="1:14" ht="45">
       <c r="A48" s="3" t="s">
         <v>124</v>
       </c>
@@ -4756,13 +4913,16 @@
         <v>135</v>
       </c>
       <c r="L48" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M48" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N48" s="1" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="49" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="49" spans="1:14" ht="60">
       <c r="A49" s="3" t="s">
         <v>125</v>
       </c>
@@ -4797,13 +4957,16 @@
         <v>135</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M49" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N49" s="1" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="50" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="50" spans="1:14" ht="60">
       <c r="A50" s="3" t="s">
         <v>126</v>
       </c>
@@ -4838,13 +5001,16 @@
         <v>135</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N50" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="51" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="51" spans="1:14" ht="75">
       <c r="A51" s="3" t="s">
         <v>127</v>
       </c>
@@ -4879,13 +5045,16 @@
         <v>135</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N51" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="52" spans="1:14" ht="45">
       <c r="A52" s="3" t="s">
         <v>128</v>
       </c>
@@ -4920,13 +5089,16 @@
         <v>135</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N52" s="1" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="53" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="53" spans="1:14" ht="45">
       <c r="A53" s="3" t="s">
         <v>37</v>
       </c>
@@ -4964,10 +5136,13 @@
         <v>135</v>
       </c>
       <c r="M53" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N53" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="54" spans="1:14" ht="60">
       <c r="A54" s="3" t="s">
         <v>38</v>
       </c>
@@ -5007,8 +5182,11 @@
       <c r="M54" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="55" spans="1:13" s="6" customFormat="1" ht="45">
+      <c r="N54" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="45">
       <c r="A55" s="3" t="s">
         <v>432</v>
       </c>
@@ -5048,8 +5226,11 @@
       <c r="M55" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="56" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N55" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="30">
       <c r="A56" s="3" t="s">
         <v>39</v>
       </c>
@@ -5089,8 +5270,11 @@
       <c r="M56" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="57" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="30">
       <c r="A57" s="3" t="s">
         <v>40</v>
       </c>
@@ -5125,13 +5309,16 @@
         <v>147</v>
       </c>
       <c r="L57" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="M57" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="N57" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="6" customFormat="1" ht="195">
+    <row r="58" spans="1:14" ht="195">
       <c r="A58" s="3" t="s">
         <v>41</v>
       </c>
@@ -5166,13 +5353,16 @@
         <v>147</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M58" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N58" s="1" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="59" spans="1:14" ht="45">
       <c r="A59" s="3" t="s">
         <v>42</v>
       </c>
@@ -5212,8 +5402,11 @@
       <c r="M59" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" s="6" customFormat="1" ht="90">
+      <c r="N59" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="90">
       <c r="A60" s="3" t="s">
         <v>43</v>
       </c>
@@ -5253,8 +5446,11 @@
       <c r="M60" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="61" spans="1:13" s="6" customFormat="1" ht="75">
+      <c r="N60" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="75">
       <c r="A61" s="3" t="s">
         <v>44</v>
       </c>
@@ -5289,13 +5485,16 @@
         <v>379</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M61" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N61" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="62" spans="1:14" ht="75">
       <c r="A62" s="3" t="s">
         <v>45</v>
       </c>
@@ -5330,13 +5529,16 @@
         <v>379</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M62" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N62" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="63" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="63" spans="1:14" ht="75">
       <c r="A63" s="3" t="s">
         <v>46</v>
       </c>
@@ -5371,13 +5573,16 @@
         <v>379</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M63" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N63" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="64" spans="1:13" s="6" customFormat="1" ht="75">
+    <row r="64" spans="1:14" ht="75">
       <c r="A64" s="3" t="s">
         <v>47</v>
       </c>
@@ -5412,13 +5617,16 @@
         <v>379</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N64" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="65" spans="1:13" s="6" customFormat="1" ht="135">
+    <row r="65" spans="1:14" ht="135">
       <c r="A65" s="3" t="s">
         <v>48</v>
       </c>
@@ -5453,13 +5661,16 @@
         <v>379</v>
       </c>
       <c r="L65" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M65" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N65" s="1" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="66" spans="1:13" s="6" customFormat="1" ht="120">
+    <row r="66" spans="1:14" ht="120">
       <c r="A66" s="3" t="s">
         <v>49</v>
       </c>
@@ -5494,13 +5705,16 @@
         <v>384</v>
       </c>
       <c r="L66" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="M66" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="M66" s="1" t="s">
+      <c r="N66" s="1" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="67" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="67" spans="1:14" ht="30">
       <c r="A67" s="3" t="s">
         <v>50</v>
       </c>
@@ -5540,8 +5754,11 @@
       <c r="M67" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" s="6" customFormat="1" ht="90">
+      <c r="N67" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="90">
       <c r="A68" s="3" t="s">
         <v>51</v>
       </c>
@@ -5581,8 +5798,11 @@
       <c r="M68" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" s="6" customFormat="1" ht="105">
+      <c r="N68" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="105">
       <c r="A69" s="3" t="s">
         <v>52</v>
       </c>
@@ -5622,8 +5842,11 @@
       <c r="M69" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="70" spans="1:13" s="6" customFormat="1" ht="75">
+      <c r="N69" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="75">
       <c r="A70" s="3" t="s">
         <v>53</v>
       </c>
@@ -5663,8 +5886,11 @@
       <c r="M70" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="71" spans="1:13" s="6" customFormat="1" ht="105">
+      <c r="N70" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="105">
       <c r="A71" s="3" t="s">
         <v>54</v>
       </c>
@@ -5704,8 +5930,11 @@
       <c r="M71" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="72" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N71" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="30">
       <c r="A72" s="3" t="s">
         <v>55</v>
       </c>
@@ -5745,8 +5974,11 @@
       <c r="M72" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="73" spans="1:13" s="6" customFormat="1" ht="60">
+      <c r="N72" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" ht="60">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -5786,8 +6018,11 @@
       <c r="M73" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" s="6" customFormat="1" ht="60">
+      <c r="N73" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" ht="60">
       <c r="A74" s="3" t="s">
         <v>57</v>
       </c>
@@ -5827,8 +6062,11 @@
       <c r="M74" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="75" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N74" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" ht="30">
       <c r="A75" s="3" t="s">
         <v>58</v>
       </c>
@@ -5863,13 +6101,16 @@
         <v>135</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M75" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="76" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N75" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" ht="30">
       <c r="A76" s="3" t="s">
         <v>59</v>
       </c>
@@ -5904,13 +6145,16 @@
         <v>135</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M76" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="77" spans="1:13" s="6" customFormat="1" ht="45">
+      <c r="N76" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" ht="45">
       <c r="A77" s="3" t="s">
         <v>60</v>
       </c>
@@ -5950,8 +6194,11 @@
       <c r="M77" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" s="6" customFormat="1" ht="60">
+      <c r="N77" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" ht="60">
       <c r="A78" s="3" t="s">
         <v>61</v>
       </c>
@@ -5986,13 +6233,16 @@
         <v>406</v>
       </c>
       <c r="L78" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M78" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N78" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="79" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="79" spans="1:14" ht="45">
       <c r="A79" s="3" t="s">
         <v>62</v>
       </c>
@@ -6027,13 +6277,16 @@
         <v>135</v>
       </c>
       <c r="L79" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M79" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N79" s="1" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="80" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="80" spans="1:14" ht="30">
       <c r="A80" s="3" t="s">
         <v>63</v>
       </c>
@@ -6068,13 +6321,16 @@
         <v>135</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M80" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N80" s="1" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="81" spans="1:14" ht="30">
       <c r="A81" s="3" t="s">
         <v>64</v>
       </c>
@@ -6114,8 +6370,11 @@
       <c r="M81" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="82" spans="1:13" s="6" customFormat="1" ht="30">
+      <c r="N81" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" ht="30">
       <c r="A82" s="3" t="s">
         <v>65</v>
       </c>
@@ -6153,10 +6412,13 @@
         <v>135</v>
       </c>
       <c r="M82" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N82" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="83" spans="1:13" s="6" customFormat="1" ht="105">
+    <row r="83" spans="1:14" ht="105">
       <c r="A83" s="3" t="s">
         <v>66</v>
       </c>
@@ -6191,13 +6453,16 @@
         <v>426</v>
       </c>
       <c r="L83" s="1" t="s">
-        <v>135</v>
+        <v>607</v>
       </c>
       <c r="M83" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N83" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="84" spans="1:13" s="6" customFormat="1" ht="105">
+    <row r="84" spans="1:14" ht="105">
       <c r="A84" s="3" t="s">
         <v>67</v>
       </c>
@@ -6235,10 +6500,13 @@
         <v>135</v>
       </c>
       <c r="M84" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N84" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="85" spans="1:14" ht="45">
       <c r="A85" s="3" t="s">
         <v>68</v>
       </c>
@@ -6276,10 +6544,13 @@
         <v>135</v>
       </c>
       <c r="M85" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N85" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="86" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="86" spans="1:14" ht="45">
       <c r="A86" s="3" t="s">
         <v>69</v>
       </c>
@@ -6314,13 +6585,16 @@
         <v>188</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M86" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N86" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="87" spans="1:13" s="6" customFormat="1" ht="120">
+    <row r="87" spans="1:14" ht="120">
       <c r="A87" s="3" t="s">
         <v>70</v>
       </c>
@@ -6355,13 +6629,16 @@
         <v>352</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M87" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N87" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="88" spans="1:14" ht="60">
       <c r="A88" s="3" t="s">
         <v>71</v>
       </c>
@@ -6396,13 +6673,16 @@
         <v>135</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M88" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N88" s="1" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="89" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="89" spans="1:14" ht="30">
       <c r="A89" s="3" t="s">
         <v>72</v>
       </c>
@@ -6437,13 +6717,16 @@
         <v>237</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M89" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N89" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="90" spans="1:13" s="6" customFormat="1" ht="120">
+    <row r="90" spans="1:14" ht="120">
       <c r="A90" s="3" t="s">
         <v>73</v>
       </c>
@@ -6478,13 +6761,16 @@
         <v>188</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M90" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N90" s="1" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="91" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="91" spans="1:14" ht="30">
       <c r="A91" s="3" t="s">
         <v>74</v>
       </c>
@@ -6519,13 +6805,16 @@
         <v>135</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M91" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N91" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="92" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="92" spans="1:14" ht="30">
       <c r="A92" s="3" t="s">
         <v>75</v>
       </c>
@@ -6560,13 +6849,16 @@
         <v>135</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M92" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N92" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="6" customFormat="1" ht="30">
+    <row r="93" spans="1:14" ht="30">
       <c r="A93" s="3" t="s">
         <v>76</v>
       </c>
@@ -6601,13 +6893,16 @@
         <v>188</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M93" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" s="6" customFormat="1" ht="60">
+      <c r="N93" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" ht="60">
       <c r="A94" s="3" t="s">
         <v>77</v>
       </c>
@@ -6642,13 +6937,16 @@
         <v>256</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M94" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N94" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="95" spans="1:13" s="6" customFormat="1" ht="60">
+    <row r="95" spans="1:14" ht="60">
       <c r="A95" s="3" t="s">
         <v>78</v>
       </c>
@@ -6683,13 +6981,16 @@
         <v>135</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>135</v>
+        <v>608</v>
       </c>
       <c r="M95" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N95" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:13" s="6" customFormat="1" ht="45">
+    <row r="96" spans="1:14" ht="45">
       <c r="A96" s="3" t="s">
         <v>79</v>
       </c>
@@ -6724,9 +7025,12 @@
         <v>135</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>135</v>
+        <v>606</v>
       </c>
       <c r="M96" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="N96" s="1" t="s">
         <v>238</v>
       </c>
     </row>

</xml_diff>